<commit_message>
mas blog y boton lateral y estilos h1 h2 h4 h4
</commit_message>
<xml_diff>
--- a/REDIRECCIONES.xlsx
+++ b/REDIRECCIONES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LACABECERA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9CB5A2-5AFB-42FC-A24F-354762289146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15AA6C6-7F74-4B7B-94ED-7BCD6F1A008B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BD0EE497-D110-4F8E-8348-3B86D9DB8E8E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="71">
   <si>
     <t>https://medicina-ayurveda.es/hernia-discal/</t>
   </si>
@@ -150,9 +150,6 @@
     <t>https://medicina-ayurveda.es/blog.html</t>
   </si>
   <si>
-    <t>https://medicina-ayurveda.es/colon-irritable.html</t>
-  </si>
-  <si>
     <t>https://medicina-ayurveda.es/difusion.html</t>
   </si>
   <si>
@@ -165,72 +162,12 @@
     <t>https://medicina-ayurveda.es/gracias.html</t>
   </si>
   <si>
-    <t>https://medicina-ayurveda.es/hernia-discal.html</t>
-  </si>
-  <si>
-    <t>https://medicina-ayurveda.es/indigestion-ajirṇa.html</t>
-  </si>
-  <si>
-    <t>https://medicina-ayurveda.es/inscripcion.html</t>
-  </si>
-  <si>
-    <t>https://medicina-ayurveda.es/kharjuradi-mantha.html</t>
-  </si>
-  <si>
-    <t>https://medicina-ayurveda.es/kichadi.html</t>
-  </si>
-  <si>
-    <t>https://medicina-ayurveda.es/menopausia-y-ayurveda.html</t>
-  </si>
-  <si>
-    <t>https://medicina-ayurveda.es/menta-piperita.html</t>
-  </si>
-  <si>
-    <t>https://medicina-ayurveda.es/politica-de-cookies.html</t>
-  </si>
-  <si>
-    <t>https://medicina-ayurveda.es/politica-de-privacidad.html</t>
-  </si>
-  <si>
-    <t>https://medicina-ayurveda.es/prakruti.html</t>
-  </si>
-  <si>
-    <t>https://medicina-ayurveda.es/prana-tejas-y-ojas.html</t>
-  </si>
-  <si>
-    <t>https://medicina-ayurveda.es/receta-de-kichadi-plato-ayurvedico.html</t>
-  </si>
-  <si>
-    <t>https://medicina-ayurveda.es/te-de-canela-y-almendras.html</t>
-  </si>
-  <si>
-    <t>https://medicina-ayurveda.es/tomando-el-pulso.html</t>
-  </si>
-  <si>
-    <t>https://medicina-ayurveda.es/yoga-nidra.html</t>
-  </si>
-  <si>
-    <t>https://medicina-ayurveda.es/zumo-de-amalaki.html</t>
-  </si>
-  <si>
     <t>https://medicina-ayurveda.es.html</t>
   </si>
   <si>
     <t>https://medicina-ayurveda.es/abhyanga-oleacion-externa.html</t>
   </si>
   <si>
-    <t>https://medicina-ayurveda.es/acne.html</t>
-  </si>
-  <si>
-    <t>https://medicina-ayurveda.es/adicciones.html</t>
-  </si>
-  <si>
-    <t>https://medicina-ayurveda.es/alergias.html</t>
-  </si>
-  <si>
-    <t>https://medicina-ayurveda.es/autismo.html</t>
-  </si>
-  <si>
     <t>https://medicina-ayurveda.es/ayurveda-online.html</t>
   </si>
   <si>
@@ -244,6 +181,72 @@
   </si>
   <si>
     <t xml:space="preserve">redireccion  a </t>
+  </si>
+  <si>
+    <t>https://medicina-ayurveda.es/blog/abhyanga-oleacion-externa.html</t>
+  </si>
+  <si>
+    <t>https://medicina-ayurveda.es/blog/acne.html</t>
+  </si>
+  <si>
+    <t>https://medicina-ayurveda.es/blog/colon-irritable.html</t>
+  </si>
+  <si>
+    <t>https://medicina-ayurveda.es/blog/hernia-discal.html</t>
+  </si>
+  <si>
+    <t>https://medicina-ayurveda.es/blog/indigestion-ajirṇa.html</t>
+  </si>
+  <si>
+    <t>https://medicina-ayurveda.es/blog/inscripcion.html</t>
+  </si>
+  <si>
+    <t>https://medicina-ayurveda.es/blog/kharjuradi-mantha.html</t>
+  </si>
+  <si>
+    <t>https://medicina-ayurveda.es/blog/kichadi.html</t>
+  </si>
+  <si>
+    <t>https://medicina-ayurveda.es/blog/menopausia-y-ayurveda.html</t>
+  </si>
+  <si>
+    <t>https://medicina-ayurveda.es/blog/menta-piperita.html</t>
+  </si>
+  <si>
+    <t>https://medicina-ayurveda.es/blog/politica-de-cookies.html</t>
+  </si>
+  <si>
+    <t>https://medicina-ayurveda.es/blog/politica-de-privacidad.html</t>
+  </si>
+  <si>
+    <t>https://medicina-ayurveda.es/blog/prakruti.html</t>
+  </si>
+  <si>
+    <t>https://medicina-ayurveda.es/blog/prana-tejas-y-ojas.html</t>
+  </si>
+  <si>
+    <t>https://medicina-ayurveda.es/blog/receta-de-kichadi-plato-ayurvedico.html</t>
+  </si>
+  <si>
+    <t>https://medicina-ayurveda.es/blog/te-de-canela-y-almendras.html</t>
+  </si>
+  <si>
+    <t>https://medicina-ayurveda.es/blog/tomando-el-pulso.html</t>
+  </si>
+  <si>
+    <t>https://medicina-ayurveda.es/blog/yoga-nidra.html</t>
+  </si>
+  <si>
+    <t>https://medicina-ayurveda.es/blog/zumo-de-amalaki.html</t>
+  </si>
+  <si>
+    <t>https://medicina-ayurveda.es/blog/adicciones.html</t>
+  </si>
+  <si>
+    <t>https://medicina-ayurveda.es/blog/alergias.html</t>
+  </si>
+  <si>
+    <t>https://medicina-ayurveda.es/blog/autismo.html</t>
   </si>
 </sst>
 </file>
@@ -614,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE129670-EB84-42D3-B2C4-4D230C95D9E0}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E36"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,10 +636,10 @@
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E1" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -645,10 +648,10 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -657,10 +660,10 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" t="s">
-        <v>60</v>
+        <v>48</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -669,10 +672,10 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" t="s">
-        <v>61</v>
+        <v>48</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -681,10 +684,10 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -693,10 +696,10 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
         <v>69</v>
-      </c>
-      <c r="E6" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -705,10 +708,10 @@
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -717,10 +720,10 @@
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E8" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -729,7 +732,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
         <v>37</v>
@@ -741,10 +744,10 @@
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" t="s">
-        <v>38</v>
+        <v>48</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -753,10 +756,10 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -765,10 +768,10 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -777,10 +780,10 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -789,10 +792,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -801,10 +804,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E15" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -813,7 +816,7 @@
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>36</v>
@@ -825,10 +828,10 @@
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -837,7 +840,7 @@
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>36</v>
@@ -849,7 +852,7 @@
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>36</v>
@@ -861,10 +864,10 @@
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -873,10 +876,10 @@
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" t="s">
-        <v>43</v>
+        <v>48</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -885,10 +888,10 @@
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" t="s">
-        <v>44</v>
+        <v>48</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -897,10 +900,10 @@
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E23" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -909,10 +912,10 @@
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E24" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -921,10 +924,10 @@
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E25" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -933,10 +936,10 @@
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E26" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -945,10 +948,10 @@
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E27" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -957,10 +960,10 @@
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E28" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -969,10 +972,10 @@
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E29" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -981,10 +984,10 @@
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E30" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -993,10 +996,10 @@
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E31" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1005,10 +1008,10 @@
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E32" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1017,10 +1020,10 @@
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E33" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1029,10 +1032,10 @@
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E34" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1041,10 +1044,10 @@
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E35" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1053,10 +1056,10 @@
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E36" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1214,8 +1217,13 @@
     <hyperlink ref="E19" r:id="rId8" xr:uid="{35D969A7-774E-49A4-A8AF-2FF411D64601}"/>
     <hyperlink ref="E11" r:id="rId9" xr:uid="{CCD59A65-3CA9-4030-8646-49BA4A04A384}"/>
     <hyperlink ref="E16" r:id="rId10" xr:uid="{0248C7D5-659C-4888-9897-CCBFE9E37046}"/>
+    <hyperlink ref="E3" r:id="rId11" xr:uid="{3B097DC7-B007-4E00-9D24-22699C401E92}"/>
+    <hyperlink ref="E4" r:id="rId12" xr:uid="{5AE1AD59-2C13-4EDF-B7AC-2C9331AFA4B6}"/>
+    <hyperlink ref="E10" r:id="rId13" xr:uid="{7254A4E6-EA10-4197-B4D6-205BDDC184E0}"/>
+    <hyperlink ref="E21" r:id="rId14" xr:uid="{44C7F2D5-B24F-4393-9AEC-9345A9A34335}"/>
+    <hyperlink ref="E22" r:id="rId15" display="https://medicina-ayurveda.es/indigestion-ajirṇa.html" xr:uid="{21D95C03-0FCF-4C5A-B716-9C060CC354F5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se ha probado el la red con fechas, visitas, likes, responisve y demas
</commit_message>
<xml_diff>
--- a/REDIRECCIONES.xlsx
+++ b/REDIRECCIONES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LACABECERA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D312CE-FDF7-4AC7-8BD2-AB5201F8AEA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452EE8BC-2311-4E61-A529-BEC2C418E00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BD0EE497-D110-4F8E-8348-3B86D9DB8E8E}"/>
+    <workbookView xWindow="3990" yWindow="1230" windowWidth="21360" windowHeight="13125" xr2:uid="{BD0EE497-D110-4F8E-8348-3B86D9DB8E8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -276,9 +276,6 @@
     <t>/blog/zumo-de-amalaki/</t>
   </si>
   <si>
-    <t>´/blog</t>
-  </si>
-  <si>
     <t>ELIMINAR</t>
   </si>
   <si>
@@ -315,7 +312,10 @@
     <t>/politica-de-cookies</t>
   </si>
   <si>
-    <t>/politica-de-privacidad</t>
+    <t>/blog/colon-irritable.html</t>
+  </si>
+  <si>
+    <t>/poliltica-de-privacidad</t>
   </si>
 </sst>
 </file>
@@ -800,7 +800,7 @@
   <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,10 +815,10 @@
         <v>5</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -826,10 +826,10 @@
         <v>6</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -837,10 +837,10 @@
         <v>16</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -851,7 +851,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -859,10 +859,10 @@
         <v>28</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -870,10 +870,10 @@
         <v>39</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -881,10 +881,10 @@
         <v>40</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -892,10 +892,10 @@
         <v>49</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -903,10 +903,10 @@
         <v>50</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -917,7 +917,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -925,10 +925,10 @@
         <v>57</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -939,7 +939,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -947,10 +947,10 @@
         <v>75</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -961,7 +961,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1027,7 +1027,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1049,7 +1049,7 @@
         <v>0</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1060,7 +1060,7 @@
         <v>0</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1093,7 +1093,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1126,7 +1126,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1137,7 +1137,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1159,7 +1159,7 @@
         <v>0</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1181,7 +1181,7 @@
         <v>0</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1203,7 +1203,7 @@
         <v>0</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1214,7 +1214,7 @@
         <v>0</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1313,7 +1313,7 @@
         <v>0</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1335,7 +1335,7 @@
         <v>0</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1346,7 +1346,7 @@
         <v>0</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1357,7 +1357,7 @@
         <v>0</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>